<commit_message>
Improved user expirience in Name Generation and Pass Generation
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Intellij\SimpleTagGen\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375C3FAD-C805-42DB-A663-5F4A9271420F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2E08BD-89BB-4320-A793-C961488CC588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="0" windowWidth="14550" windowHeight="11295" xr2:uid="{1935E06E-31D0-441F-A3D5-9089803FC850}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1935E06E-31D0-441F-A3D5-9089803FC850}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1250,8 +1250,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,7 +2533,7 @@
         <v>132</v>
       </c>
       <c r="F56" s="21">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="G56" s="21">
         <v>120</v>
@@ -2556,7 +2556,7 @@
         <v>132</v>
       </c>
       <c r="F57" s="21">
-        <v>114</v>
+        <v>950</v>
       </c>
       <c r="G57" s="21">
         <v>480</v>
@@ -2797,7 +2797,7 @@
         <v>137</v>
       </c>
       <c r="F68" s="23">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="G68" s="23">
         <v>140</v>
@@ -2820,10 +2820,10 @@
         <v>137</v>
       </c>
       <c r="F69" s="23">
+        <v>146</v>
+      </c>
+      <c r="G69" s="23">
         <v>100</v>
-      </c>
-      <c r="G69" s="23">
-        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2843,10 +2843,10 @@
         <v>137</v>
       </c>
       <c r="F70" s="23">
+        <v>120</v>
+      </c>
+      <c r="G70" s="23">
         <v>160</v>
-      </c>
-      <c r="G70" s="23">
-        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2866,10 +2866,10 @@
         <v>137</v>
       </c>
       <c r="F71" s="23">
+        <v>118</v>
+      </c>
+      <c r="G71" s="23">
         <v>160</v>
-      </c>
-      <c r="G71" s="23">
-        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2889,10 +2889,10 @@
         <v>137</v>
       </c>
       <c r="F72" s="23">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G72" s="23">
-        <v>138</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>